<commit_message>
fixed red flag bug
</commit_message>
<xml_diff>
--- a/koalifications.xlsx
+++ b/koalifications.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/theochiu/Documents/GitHub/datetrix/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Theodore Chiu\Documents\Github\datetrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0BE3A91-C29F-3F4E-9E3B-601D586EB5CC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE2DCA0-10E5-4EF5-9C10-E11E43809951}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16140" xr2:uid="{B495A9EA-6FC0-C14E-84FB-A63439172DAA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B495A9EA-6FC0-C14E-84FB-A63439172DAA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -844,18 +844,18 @@
   <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="33.6640625" customWidth="1"/>
+    <col min="1" max="1" width="33.625" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="23.1640625" customWidth="1"/>
+    <col min="3" max="3" width="23.125" customWidth="1"/>
     <col min="4" max="4" width="54" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25">
+    <row r="1" spans="1:4" ht="23.25">
       <c r="A1" s="13" t="s">
         <v>53</v>
       </c>
@@ -869,7 +869,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17">
+    <row r="2" spans="1:4">
       <c r="A2" s="16" t="s">
         <v>2</v>
       </c>
@@ -881,7 +881,7 @@
       </c>
       <c r="D2" s="12"/>
     </row>
-    <row r="3" spans="1:4" ht="17">
+    <row r="3" spans="1:4">
       <c r="A3" s="16" t="s">
         <v>4</v>
       </c>
@@ -895,7 +895,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17">
+    <row r="4" spans="1:4">
       <c r="A4" s="16" t="s">
         <v>6</v>
       </c>
@@ -907,7 +907,7 @@
       </c>
       <c r="D4" s="12"/>
     </row>
-    <row r="5" spans="1:4" ht="17">
+    <row r="5" spans="1:4">
       <c r="A5" s="16" t="s">
         <v>7</v>
       </c>
@@ -921,7 +921,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="17">
+    <row r="6" spans="1:4">
       <c r="A6" s="16" t="s">
         <v>8</v>
       </c>
@@ -935,7 +935,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="17">
+    <row r="7" spans="1:4">
       <c r="A7" s="16" t="s">
         <v>58</v>
       </c>
@@ -949,7 +949,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="17">
+    <row r="8" spans="1:4">
       <c r="A8" s="16" t="s">
         <v>39</v>
       </c>
@@ -977,7 +977,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="17">
+    <row r="10" spans="1:4">
       <c r="A10" s="16" t="s">
         <v>12</v>
       </c>
@@ -989,7 +989,7 @@
       </c>
       <c r="D10" s="12"/>
     </row>
-    <row r="11" spans="1:4" ht="17">
+    <row r="11" spans="1:4">
       <c r="A11" s="16" t="s">
         <v>13</v>
       </c>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="D11" s="12"/>
     </row>
-    <row r="12" spans="1:4" ht="17">
+    <row r="12" spans="1:4">
       <c r="A12" s="16" t="s">
         <v>14</v>
       </c>
@@ -1009,11 +1009,11 @@
         <v>15</v>
       </c>
       <c r="C12" s="17">
-        <v>1000</v>
+        <v>-1</v>
       </c>
       <c r="D12" s="12"/>
     </row>
-    <row r="13" spans="1:4" ht="17">
+    <row r="13" spans="1:4">
       <c r="A13" s="16" t="s">
         <v>16</v>
       </c>
@@ -1025,7 +1025,7 @@
       </c>
       <c r="D13" s="12"/>
     </row>
-    <row r="14" spans="1:4" ht="17">
+    <row r="14" spans="1:4">
       <c r="A14" s="16" t="s">
         <v>17</v>
       </c>
@@ -1037,7 +1037,7 @@
       </c>
       <c r="D14" s="12"/>
     </row>
-    <row r="15" spans="1:4" ht="17">
+    <row r="15" spans="1:4">
       <c r="A15" s="16" t="s">
         <v>18</v>
       </c>
@@ -1049,7 +1049,7 @@
       </c>
       <c r="D15" s="12"/>
     </row>
-    <row r="16" spans="1:4" ht="17">
+    <row r="16" spans="1:4">
       <c r="A16" s="16" t="s">
         <v>19</v>
       </c>
@@ -1061,7 +1061,7 @@
       </c>
       <c r="D16" s="12"/>
     </row>
-    <row r="17" spans="1:4" ht="17">
+    <row r="17" spans="1:4">
       <c r="A17" s="16" t="s">
         <v>20</v>
       </c>
@@ -1073,7 +1073,7 @@
       </c>
       <c r="D17" s="12"/>
     </row>
-    <row r="18" spans="1:4" ht="17">
+    <row r="18" spans="1:4">
       <c r="A18" s="16" t="s">
         <v>21</v>
       </c>
@@ -1085,7 +1085,7 @@
       </c>
       <c r="D18" s="12"/>
     </row>
-    <row r="19" spans="1:4" ht="17">
+    <row r="19" spans="1:4">
       <c r="A19" s="16" t="s">
         <v>22</v>
       </c>
@@ -1097,7 +1097,7 @@
       </c>
       <c r="D19" s="12"/>
     </row>
-    <row r="20" spans="1:4" ht="17">
+    <row r="20" spans="1:4">
       <c r="A20" s="16" t="s">
         <v>23</v>
       </c>
@@ -1109,7 +1109,7 @@
       </c>
       <c r="D20" s="12"/>
     </row>
-    <row r="21" spans="1:4" ht="17">
+    <row r="21" spans="1:4">
       <c r="A21" s="16" t="s">
         <v>26</v>
       </c>
@@ -1121,7 +1121,7 @@
       </c>
       <c r="D21" s="12"/>
     </row>
-    <row r="22" spans="1:4" ht="17">
+    <row r="22" spans="1:4">
       <c r="A22" s="16" t="s">
         <v>49</v>
       </c>
@@ -1135,7 +1135,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17">
+    <row r="23" spans="1:4">
       <c r="A23" s="16" t="s">
         <v>46</v>
       </c>
@@ -1149,7 +1149,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17">
+    <row r="24" spans="1:4">
       <c r="A24" s="16" t="s">
         <v>36</v>
       </c>
@@ -1163,7 +1163,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17">
+    <row r="25" spans="1:4">
       <c r="A25" s="9" t="s">
         <v>43</v>
       </c>
@@ -1177,7 +1177,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17">
+    <row r="26" spans="1:4">
       <c r="A26" s="9" t="s">
         <v>50</v>
       </c>
@@ -1191,7 +1191,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="17">
+    <row r="27" spans="1:4">
       <c r="A27" s="9" t="s">
         <v>52</v>
       </c>
@@ -1203,7 +1203,7 @@
       </c>
       <c r="D27" s="11"/>
     </row>
-    <row r="28" spans="1:4" ht="17">
+    <row r="28" spans="1:4">
       <c r="A28" s="9" t="s">
         <v>54</v>
       </c>
@@ -1215,7 +1215,7 @@
       </c>
       <c r="D28" s="11"/>
     </row>
-    <row r="29" spans="1:4" ht="34">
+    <row r="29" spans="1:4" ht="31.5">
       <c r="A29" s="9" t="s">
         <v>55</v>
       </c>
@@ -1229,7 +1229,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="17">
+    <row r="30" spans="1:4">
       <c r="A30" s="9" t="s">
         <v>60</v>
       </c>
@@ -1243,7 +1243,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="34">
+    <row r="31" spans="1:4">
       <c r="A31" s="9" t="s">
         <v>62</v>
       </c>
@@ -1255,7 +1255,7 @@
       </c>
       <c r="D31" s="11"/>
     </row>
-    <row r="32" spans="1:4" ht="17">
+    <row r="32" spans="1:4">
       <c r="A32" s="9" t="s">
         <v>59</v>
       </c>
@@ -1267,7 +1267,7 @@
       </c>
       <c r="D32" s="11"/>
     </row>
-    <row r="33" spans="1:4" ht="17">
+    <row r="33" spans="1:4">
       <c r="A33" s="9" t="s">
         <v>65</v>
       </c>
@@ -1281,7 +1281,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="17">
+    <row r="34" spans="1:4">
       <c r="A34" s="9" t="s">
         <v>67</v>
       </c>
@@ -1293,7 +1293,7 @@
       </c>
       <c r="D34" s="11"/>
     </row>
-    <row r="35" spans="1:4" ht="17">
+    <row r="35" spans="1:4">
       <c r="A35" s="9" t="s">
         <v>63</v>
       </c>
@@ -1307,7 +1307,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="18" thickBot="1">
+    <row r="36" spans="1:4" ht="16.5" thickBot="1">
       <c r="A36" s="19" t="s">
         <v>30</v>
       </c>
@@ -1327,13 +1327,13 @@
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
     </row>
-    <row r="38" spans="1:4" ht="17">
+    <row r="38" spans="1:4">
       <c r="A38" s="22" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="17" thickBot="1"/>
-    <row r="40" spans="1:4" ht="24">
+    <row r="39" spans="1:4" ht="16.5" thickBot="1"/>
+    <row r="40" spans="1:4" ht="23.25">
       <c r="B40" s="2" t="s">
         <v>32</v>
       </c>
@@ -1341,7 +1341,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="24">
+    <row r="41" spans="1:4" ht="23.25">
       <c r="B41" s="4" t="s">
         <v>33</v>
       </c>
@@ -1372,7 +1372,7 @@
       </c>
       <c r="C45" s="5"/>
     </row>
-    <row r="46" spans="1:4" ht="17" thickBot="1">
+    <row r="46" spans="1:4" ht="16.5" thickBot="1">
       <c r="B46" s="6" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
played with weights, updated spreadsheet
</commit_message>
<xml_diff>
--- a/koalifications.xlsx
+++ b/koalifications.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Theodore Chiu\Documents\Github\datetrix\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/theochiu/Documents/GitHub/datetrix/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04C84F7F-A61B-4EEC-A127-44D7FBF93572}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12817CF-247D-A64A-B510-D30B2F0778C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B495A9EA-6FC0-C14E-84FB-A63439172DAA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{B495A9EA-6FC0-C14E-84FB-A63439172DAA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="74">
   <si>
     <t>Importance</t>
   </si>
@@ -241,13 +241,25 @@
   </si>
   <si>
     <t>&gt;=84 +- 2</t>
+  </si>
+  <si>
+    <t>the -1 for parsing</t>
+  </si>
+  <si>
+    <t>wants kids</t>
+  </si>
+  <si>
+    <t>Psalm 127:4</t>
+  </si>
+  <si>
+    <t>genuine</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -841,21 +853,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D48305B0-C1F0-B743-AFB6-D5D38718AEB1}">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="150" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.625" customWidth="1"/>
+    <col min="1" max="1" width="33.6640625" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="23.125" customWidth="1"/>
+    <col min="3" max="3" width="23.1640625" customWidth="1"/>
     <col min="4" max="4" width="54" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="23.25">
+    <row r="1" spans="1:4" ht="25" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>53</v>
       </c>
@@ -869,7 +881,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>2</v>
       </c>
@@ -877,11 +889,11 @@
         <v>3</v>
       </c>
       <c r="C2" s="17">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D2" s="12"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
         <v>4</v>
       </c>
@@ -889,13 +901,13 @@
         <v>5</v>
       </c>
       <c r="C3" s="17">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>6</v>
       </c>
@@ -903,11 +915,11 @@
         <v>10</v>
       </c>
       <c r="C4" s="17">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D4" s="12"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>7</v>
       </c>
@@ -915,13 +927,13 @@
         <v>9</v>
       </c>
       <c r="C5" s="17">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
         <v>8</v>
       </c>
@@ -929,13 +941,13 @@
         <v>9</v>
       </c>
       <c r="C6" s="17">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
         <v>58</v>
       </c>
@@ -943,13 +955,13 @@
         <v>5</v>
       </c>
       <c r="C7" s="17">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
         <v>39</v>
       </c>
@@ -963,7 +975,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="33" customHeight="1">
+    <row r="9" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
         <v>11</v>
       </c>
@@ -977,7 +989,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
         <v>12</v>
       </c>
@@ -989,7 +1001,7 @@
       </c>
       <c r="D10" s="12"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
         <v>13</v>
       </c>
@@ -997,11 +1009,11 @@
         <v>10</v>
       </c>
       <c r="C11" s="17">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="D11" s="12"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
         <v>14</v>
       </c>
@@ -1011,9 +1023,11 @@
       <c r="C12" s="17">
         <v>-1</v>
       </c>
-      <c r="D12" s="12"/>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="D12" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
         <v>16</v>
       </c>
@@ -1025,7 +1039,7 @@
       </c>
       <c r="D13" s="12"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>17</v>
       </c>
@@ -1033,11 +1047,11 @@
         <v>9</v>
       </c>
       <c r="C14" s="17">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D14" s="12"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
         <v>18</v>
       </c>
@@ -1049,7 +1063,7 @@
       </c>
       <c r="D15" s="12"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="s">
         <v>19</v>
       </c>
@@ -1057,11 +1071,11 @@
         <v>15</v>
       </c>
       <c r="C16" s="17">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D16" s="12"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
         <v>20</v>
       </c>
@@ -1069,11 +1083,11 @@
         <v>10</v>
       </c>
       <c r="C17" s="17">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="D17" s="12"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="s">
         <v>21</v>
       </c>
@@ -1085,7 +1099,7 @@
       </c>
       <c r="D18" s="12"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
         <v>22</v>
       </c>
@@ -1097,7 +1111,7 @@
       </c>
       <c r="D19" s="12"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="16" t="s">
         <v>23</v>
       </c>
@@ -1109,7 +1123,7 @@
       </c>
       <c r="D20" s="12"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="16" t="s">
         <v>26</v>
       </c>
@@ -1121,7 +1135,7 @@
       </c>
       <c r="D21" s="12"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="16" t="s">
         <v>49</v>
       </c>
@@ -1129,13 +1143,13 @@
         <v>10</v>
       </c>
       <c r="C22" s="17">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D22" s="12" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="16" t="s">
         <v>46</v>
       </c>
@@ -1143,13 +1157,13 @@
         <v>9</v>
       </c>
       <c r="C23" s="17">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D23" s="12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="16" t="s">
         <v>36</v>
       </c>
@@ -1163,7 +1177,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
         <v>43</v>
       </c>
@@ -1171,13 +1185,13 @@
         <v>10</v>
       </c>
       <c r="C25" s="10">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D25" s="11" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
         <v>50</v>
       </c>
@@ -1191,7 +1205,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
         <v>52</v>
       </c>
@@ -1203,7 +1217,7 @@
       </c>
       <c r="D27" s="11"/>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
         <v>54</v>
       </c>
@@ -1215,7 +1229,7 @@
       </c>
       <c r="D28" s="11"/>
     </row>
-    <row r="29" spans="1:4" ht="31.5">
+    <row r="29" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
         <v>55</v>
       </c>
@@ -1229,7 +1243,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
         <v>60</v>
       </c>
@@ -1243,7 +1257,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
         <v>61</v>
       </c>
@@ -1255,7 +1269,7 @@
       </c>
       <c r="D31" s="11"/>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
         <v>59</v>
       </c>
@@ -1267,12 +1281,12 @@
       </c>
       <c r="D32" s="11"/>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
         <v>64</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>9</v>
+        <v>67</v>
       </c>
       <c r="C33" s="10">
         <v>15</v>
@@ -1281,7 +1295,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
         <v>66</v>
       </c>
@@ -1293,7 +1307,7 @@
       </c>
       <c r="D34" s="11"/>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
         <v>62</v>
       </c>
@@ -1307,83 +1321,115 @@
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="16.5" thickBot="1">
-      <c r="A36" s="19" t="s">
+    <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" s="10">
+        <v>25</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="9"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="11"/>
+    </row>
+    <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" s="10">
+        <v>40</v>
+      </c>
+      <c r="D38" s="11"/>
+    </row>
+    <row r="39" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="B36" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C36" s="20">
+      <c r="B39" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="20">
         <v>30</v>
       </c>
-      <c r="D36" s="21" t="s">
+      <c r="D39" s="21" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="8"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="22" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="8"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+    </row>
+    <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A41" s="22" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="16.5" thickBot="1"/>
-    <row r="40" spans="1:4" ht="23.25">
-      <c r="B40" s="2" t="s">
+    <row r="42" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:4" ht="24" x14ac:dyDescent="0.3">
+      <c r="B43" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C43" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="23.25">
-      <c r="B41" s="4" t="s">
+    <row r="44" spans="1:4" ht="24" x14ac:dyDescent="0.3">
+      <c r="B44" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C41" s="5"/>
-      <c r="D41" s="1"/>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="B42" s="4" t="s">
+      <c r="C44" s="5"/>
+      <c r="D44" s="1"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B45" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C42" s="5"/>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="B43" s="4" t="s">
+      <c r="C45" s="5"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B46" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C43" s="5"/>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="B44" s="4" t="s">
+      <c r="C46" s="5"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B47" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C44" s="5"/>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="B45" s="4" t="s">
+      <c r="C47" s="5"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B48" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C45" s="5"/>
-    </row>
-    <row r="46" spans="1:4" ht="16.5" thickBot="1">
-      <c r="B46" s="6" t="s">
+      <c r="C48" s="5"/>
+    </row>
+    <row r="49" spans="2:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C46" s="7" t="s">
+      <c r="C49" s="7" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D44">
+  <conditionalFormatting sqref="D47">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="high">
-      <formula>NOT(ISERROR(SEARCH("high",D44)))</formula>
+      <formula>NOT(ISERROR(SEARCH("high",D47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>